<commit_message>
Add Unlevered FCF and Sensitivity Revenue Analysis
</commit_message>
<xml_diff>
--- a/SaaSV/SaaSV_model_v2.xlsx
+++ b/SaaSV/SaaSV_model_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\quant-summer-2025\SaaSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A64639-D5CC-471E-9EBF-A366E98BA97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333D6588-4E10-428C-8863-48182915BAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" activeTab="4" xr2:uid="{270BAFE9-F160-4EC3-8ED5-C7005A9C532B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{270BAFE9-F160-4EC3-8ED5-C7005A9C532B}"/>
   </bookViews>
   <sheets>
     <sheet name="Drivers" sheetId="1" r:id="rId1"/>
@@ -226,15 +226,15 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0,"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0,;\(&quot;$&quot;#,##0,\)"/>
-    <numFmt numFmtId="172" formatCode="\F\C\F\ &quot;2024&quot;"/>
-    <numFmt numFmtId="173" formatCode="\F\C\F\ &quot;2025&quot;"/>
-    <numFmt numFmtId="174" formatCode="&quot;Bull (+5%)&quot;"/>
-    <numFmt numFmtId="175" formatCode="&quot;Base&quot;"/>
-    <numFmt numFmtId="176" formatCode="&quot;Bear (-5%)&quot;"/>
-    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,###,"/>
-    <numFmt numFmtId="178" formatCode="&quot;FCF 2026&quot;"/>
-    <numFmt numFmtId="179" formatCode="\F\C\F\ &quot;2028&quot;"/>
-    <numFmt numFmtId="180" formatCode="&quot;FCF 2027&quot;"/>
+    <numFmt numFmtId="167" formatCode="\F\C\F\ &quot;2024&quot;"/>
+    <numFmt numFmtId="168" formatCode="\F\C\F\ &quot;2025&quot;"/>
+    <numFmt numFmtId="169" formatCode="&quot;Bull (+5%)&quot;"/>
+    <numFmt numFmtId="170" formatCode="&quot;Base&quot;"/>
+    <numFmt numFmtId="171" formatCode="&quot;Bear (-5%)&quot;"/>
+    <numFmt numFmtId="172" formatCode="&quot;$&quot;#,###,"/>
+    <numFmt numFmtId="173" formatCode="&quot;FCF 2026&quot;"/>
+    <numFmt numFmtId="174" formatCode="\F\C\F\ &quot;2028&quot;"/>
+    <numFmt numFmtId="175" formatCode="&quot;FCF 2027&quot;"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -414,40 +414,40 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="174" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="175" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="179" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -840,10 +840,10 @@
         <f t="shared" si="0"/>
         <v>2936.2500000000005</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="36"/>
+      <c r="I2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -864,8 +864,8 @@
       <c r="F3" s="21">
         <v>0.2</v>
       </c>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
     </row>
     <row r="4" spans="1:10" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -1086,7 +1086,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="B15" s="38"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1168,10 +1168,10 @@
         <v>13219100.973450003</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="37"/>
+      <c r="I2" s="50"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -1198,8 +1198,8 @@
         <v>-264382.01946900005</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
@@ -1226,8 +1226,8 @@
         <v>12954718.953981003</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -1254,10 +1254,10 @@
         <v>-2776011.2044245</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="36"/>
+      <c r="I5" s="49"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -1284,8 +1284,8 @@
         <v>-1850674.136283</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
@@ -1489,10 +1489,10 @@
         <f>CashFlow!E14</f>
         <v>11896077.326106068</v>
       </c>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="37"/>
+      <c r="I2" s="50"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -1518,8 +1518,8 @@
         <f>IncomeStmt!F$2/365*Drivers!F$11</f>
         <v>1484885.3148258908</v>
       </c>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1540,8 +1540,8 @@
       <c r="F4" s="23">
         <v>50000</v>
       </c>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
@@ -1567,10 +1567,10 @@
         <f t="shared" si="0"/>
         <v>13430962.640931958</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="36"/>
+      <c r="I5" s="49"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -1596,8 +1596,8 @@
         <f>-(IncomeStmt!F$3/365)*Drivers!F$12</f>
         <v>21730.02899745206</v>
       </c>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -1712,10 +1712,10 @@
         <f>IncomeStmt!F11</f>
         <v>6246025.209955127</v>
       </c>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="37"/>
+      <c r="I2" s="50"/>
     </row>
     <row r="3" spans="1:9" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -1736,8 +1736,8 @@
       <c r="F3" s="27">
         <v>0</v>
       </c>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -1763,8 +1763,8 @@
         <f>-1*(BalanceSheet!G3-BalanceSheet!F3)</f>
         <v>1484885.3148258908</v>
       </c>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1790,10 +1790,10 @@
         <f>BalanceSheet!G6-BalanceSheet!F6</f>
         <v>-21730.02899745206</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="36"/>
+      <c r="I5" s="49"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
@@ -1819,8 +1819,8 @@
         <f t="shared" si="0"/>
         <v>7709180.4957835656</v>
       </c>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
     </row>
     <row r="7" spans="1:9" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -2141,10 +2141,10 @@
         <v>2082008.4033183756</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="37" t="s">
+      <c r="H3" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="37"/>
+      <c r="I3" s="50"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -2172,8 +2172,8 @@
         <v>264382.01946900005</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -2201,8 +2201,8 @@
         <v>264382.01946900005</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -2230,10 +2230,10 @@
         <v>1463155.2858284388</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="36" t="s">
+      <c r="H6" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="36"/>
+      <c r="I6" s="49"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2261,8 +2261,8 @@
         <v>4782869.9241266884</v>
       </c>
       <c r="G7" s="1"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -2278,41 +2278,41 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="H9" s="43" t="s">
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="H9" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="I9" s="49">
+      <c r="I9" s="46">
         <v>1</v>
       </c>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="45"/>
-      <c r="B10" s="46">
+      <c r="A10" s="42"/>
+      <c r="B10" s="43">
         <f>B7</f>
         <v>1873757.8082191781</v>
       </c>
-      <c r="C10" s="47">
+      <c r="C10" s="44">
         <f>C7</f>
         <v>2808511.610410959</v>
       </c>
-      <c r="D10" s="48">
+      <c r="D10" s="45">
         <f>D7</f>
         <v>3923904.179465754</v>
       </c>
-      <c r="E10" s="51">
+      <c r="E10" s="48">
         <f>E7</f>
         <v>5143063.6147355465</v>
       </c>
-      <c r="F10" s="50">
+      <c r="F10" s="47">
         <f>F7</f>
         <v>4782869.9241266884</v>
       </c>
@@ -2321,23 +2321,23 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="39">
+      <c r="A11" s="37">
         <v>1.05</v>
       </c>
-      <c r="B11" s="42">
+      <c r="B11" s="40">
         <f t="dataTable" ref="B11:F13" dt2D="0" dtr="0" r1="I9"/>
         <v>1967445.6986301369</v>
       </c>
-      <c r="C11" s="42">
+      <c r="C11" s="40">
         <v>2948937.1909315069</v>
       </c>
-      <c r="D11" s="42">
+      <c r="D11" s="40">
         <v>4120099.388439042</v>
       </c>
-      <c r="E11" s="42">
+      <c r="E11" s="40">
         <v>5400216.7954723239</v>
       </c>
-      <c r="F11" s="42">
+      <c r="F11" s="40">
         <v>5022013.4203330241</v>
       </c>
       <c r="G11" s="1"/>
@@ -2346,42 +2346,42 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="40">
+      <c r="A12" s="38">
         <v>1</v>
       </c>
-      <c r="B12" s="42">
+      <c r="B12" s="40">
         <v>1873757.8082191781</v>
       </c>
-      <c r="C12" s="42">
+      <c r="C12" s="40">
         <v>2808511.610410959</v>
       </c>
-      <c r="D12" s="42">
+      <c r="D12" s="40">
         <v>3923904.179465754</v>
       </c>
-      <c r="E12" s="42">
+      <c r="E12" s="40">
         <v>5143063.6147355465</v>
       </c>
-      <c r="F12" s="42">
+      <c r="F12" s="40">
         <v>4782869.9241266884</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="41">
+      <c r="A13" s="39">
         <v>0.95</v>
       </c>
-      <c r="B13" s="42">
+      <c r="B13" s="40">
         <v>1780069.9178082191</v>
       </c>
-      <c r="C13" s="42">
+      <c r="C13" s="40">
         <v>2668086.0298904111</v>
       </c>
-      <c r="D13" s="42">
+      <c r="D13" s="40">
         <v>3727708.9704924664</v>
       </c>
-      <c r="E13" s="42">
+      <c r="E13" s="40">
         <v>4885910.4339987701</v>
       </c>
-      <c r="F13" s="42">
+      <c r="F13" s="40">
         <v>4543726.4279203527</v>
       </c>
     </row>

</xml_diff>